<commit_message>
Latest version with docker files
</commit_message>
<xml_diff>
--- a/scCRISPR_suppFiles/Amplicon_primer_sheet.xlsx
+++ b/scCRISPR_suppFiles/Amplicon_primer_sheet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="149">
   <si>
     <t xml:space="preserve">Chromosome</t>
   </si>
@@ -44,6 +44,9 @@
   </si>
   <si>
     <t xml:space="preserve">AMP_Edite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Primer_Ident</t>
   </si>
   <si>
     <t xml:space="preserve">chr9</t>
@@ -701,13 +704,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H41"/>
+  <dimension ref="A1:J41"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L19" activeCellId="0" sqref="L19"/>
+      <selection pane="topLeft" activeCell="M28" activeCellId="0" sqref="M28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.49"/>
@@ -716,7 +719,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -741,36 +744,44 @@
       <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2"/>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" s="4" t="n">
         <v>53503999</v>
       </c>
       <c r="C2" s="4" t="n">
-        <v>53504219</v>
+        <v>53504218</v>
       </c>
       <c r="D2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="4" t="n">
+        <v>90</v>
+      </c>
+      <c r="J2" s="4"/>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="6" t="s">
         <v>9</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="s">
-        <v>8</v>
       </c>
       <c r="B3" s="6" t="n">
         <v>7861126</v>
@@ -779,24 +790,28 @@
         <v>7861370</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>14</v>
+      </c>
+      <c r="I3" s="4" t="n">
+        <v>90</v>
+      </c>
+      <c r="J3" s="4"/>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B4" s="4" t="n">
         <v>73504966</v>
@@ -805,24 +820,28 @@
         <v>73505193</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>14</v>
+      </c>
+      <c r="I4" s="4" t="n">
+        <v>90</v>
+      </c>
+      <c r="J4" s="4"/>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B5" s="6" t="n">
         <v>119903179</v>
@@ -831,24 +850,28 @@
         <v>119903402</v>
       </c>
       <c r="D5" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" s="4" t="n">
+        <v>90</v>
+      </c>
+      <c r="J5" s="4"/>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
-        <v>21</v>
       </c>
       <c r="B6" s="4" t="n">
         <v>157134898</v>
@@ -857,24 +880,28 @@
         <v>157135130</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>14</v>
+      </c>
+      <c r="I6" s="4" t="n">
+        <v>90</v>
+      </c>
+      <c r="J6" s="4"/>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B7" s="6" t="n">
         <v>69588472</v>
@@ -883,24 +910,28 @@
         <v>69588675</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>14</v>
+      </c>
+      <c r="I7" s="4" t="n">
+        <v>100</v>
+      </c>
+      <c r="J7" s="4"/>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B8" s="4" t="n">
         <v>82642300</v>
@@ -909,24 +940,28 @@
         <v>82642514</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>14</v>
+      </c>
+      <c r="I8" s="4" t="n">
+        <v>90</v>
+      </c>
+      <c r="J8" s="4"/>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B9" s="6" t="n">
         <v>42752482</v>
@@ -935,24 +970,28 @@
         <v>42752700</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>14</v>
+      </c>
+      <c r="I9" s="4" t="n">
+        <v>90</v>
+      </c>
+      <c r="J9" s="4"/>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B10" s="4" t="n">
         <v>139775591</v>
@@ -961,24 +1000,28 @@
         <v>139775850</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>14</v>
+      </c>
+      <c r="I10" s="4" t="n">
+        <v>90</v>
+      </c>
+      <c r="J10" s="4"/>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B11" s="6" t="n">
         <v>118462594</v>
@@ -987,24 +1030,28 @@
         <v>118462792</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>14</v>
+      </c>
+      <c r="I11" s="4" t="n">
+        <v>90</v>
+      </c>
+      <c r="J11" s="4"/>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B12" s="4" t="n">
         <v>163469484</v>
@@ -1013,24 +1060,28 @@
         <v>163469692</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>14</v>
+      </c>
+      <c r="I12" s="4" t="n">
+        <v>90</v>
+      </c>
+      <c r="J12" s="4"/>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B13" s="6" t="n">
         <v>96688487</v>
@@ -1039,24 +1090,28 @@
         <v>96688706</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>14</v>
+      </c>
+      <c r="I13" s="4" t="n">
+        <v>90</v>
+      </c>
+      <c r="J13" s="4"/>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B14" s="4" t="n">
         <v>76521668</v>
@@ -1065,24 +1120,28 @@
         <v>76521914</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>14</v>
+      </c>
+      <c r="I14" s="4" t="n">
+        <v>90</v>
+      </c>
+      <c r="J14" s="4"/>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B15" s="6" t="n">
         <v>137278352</v>
@@ -1091,24 +1150,28 @@
         <v>137278575</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>14</v>
+      </c>
+      <c r="I15" s="4" t="n">
+        <v>90</v>
+      </c>
+      <c r="J15" s="4"/>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B16" s="4" t="n">
         <v>54420138</v>
@@ -1117,24 +1180,28 @@
         <v>54420372</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>14</v>
+      </c>
+      <c r="I16" s="4" t="n">
+        <v>100</v>
+      </c>
+      <c r="J16" s="4"/>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B17" s="6" t="n">
         <v>106237472</v>
@@ -1143,24 +1210,28 @@
         <v>106237679</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>14</v>
+      </c>
+      <c r="I17" s="4" t="n">
+        <v>90</v>
+      </c>
+      <c r="J17" s="4"/>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B18" s="4" t="n">
         <v>21516707</v>
@@ -1169,24 +1240,28 @@
         <v>21516909</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>14</v>
+      </c>
+      <c r="I18" s="4" t="n">
+        <v>90</v>
+      </c>
+      <c r="J18" s="4"/>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B19" s="6" t="n">
         <v>134664103</v>
@@ -1195,24 +1270,28 @@
         <v>134664322</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>14</v>
+      </c>
+      <c r="I19" s="4" t="n">
+        <v>90</v>
+      </c>
+      <c r="J19" s="4"/>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B20" s="4" t="n">
         <v>108533831</v>
@@ -1221,24 +1300,28 @@
         <v>108534045</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>14</v>
+      </c>
+      <c r="I20" s="4" t="n">
+        <v>90</v>
+      </c>
+      <c r="J20" s="4"/>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B21" s="6" t="n">
         <v>122970841</v>
@@ -1247,24 +1330,28 @@
         <v>122971065</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>14</v>
+      </c>
+      <c r="I21" s="4" t="n">
+        <v>90</v>
+      </c>
+      <c r="J21" s="4"/>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B22" s="4" t="n">
         <v>80239685</v>
@@ -1273,24 +1360,28 @@
         <v>80239927</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>14</v>
+      </c>
+      <c r="I22" s="4" t="n">
+        <v>90</v>
+      </c>
+      <c r="J22" s="4"/>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="6" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B23" s="6" t="n">
         <v>88174649</v>
@@ -1299,24 +1390,28 @@
         <v>88174872</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>14</v>
+      </c>
+      <c r="I23" s="4" t="n">
+        <v>90</v>
+      </c>
+      <c r="J23" s="4"/>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B24" s="4" t="n">
         <v>19887627</v>
@@ -1325,24 +1420,28 @@
         <v>19887869</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>14</v>
+      </c>
+      <c r="I24" s="4" t="n">
+        <v>90</v>
+      </c>
+      <c r="J24" s="4"/>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="6" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B25" s="6" t="n">
         <v>119908556</v>
@@ -1351,24 +1450,28 @@
         <v>119908789</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>14</v>
+      </c>
+      <c r="I25" s="4" t="n">
+        <v>90</v>
+      </c>
+      <c r="J25" s="4"/>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="4" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B26" s="4" t="n">
         <v>122247491</v>
@@ -1377,24 +1480,28 @@
         <v>122247722</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>14</v>
+      </c>
+      <c r="I26" s="4" t="n">
+        <v>90</v>
+      </c>
+      <c r="J26" s="4"/>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B27" s="6" t="n">
         <v>44922323</v>
@@ -1403,24 +1510,28 @@
         <v>44922546</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>14</v>
+      </c>
+      <c r="I27" s="4" t="n">
+        <v>90</v>
+      </c>
+      <c r="J27" s="4"/>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B28" s="4" t="n">
         <v>38970783</v>
@@ -1429,24 +1540,28 @@
         <v>38971022</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>14</v>
+      </c>
+      <c r="I28" s="4" t="n">
+        <v>90</v>
+      </c>
+      <c r="J28" s="4"/>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="6" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B29" s="6" t="n">
         <v>49068040</v>
@@ -1455,24 +1570,28 @@
         <v>49068299</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>14</v>
+      </c>
+      <c r="I29" s="4" t="n">
+        <v>90</v>
+      </c>
+      <c r="J29" s="4"/>
+    </row>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="4" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B30" s="4" t="n">
         <v>106194330</v>
@@ -1481,24 +1600,28 @@
         <v>106194565</v>
       </c>
       <c r="D30" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="E30" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="H30" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="I30" s="4" t="n">
+        <v>90</v>
+      </c>
+      <c r="J30" s="4"/>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="6" t="s">
         <v>110</v>
-      </c>
-      <c r="E30" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="G30" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="H30" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="6" t="s">
-        <v>109</v>
       </c>
       <c r="B31" s="6" t="n">
         <v>106196773</v>
@@ -1507,24 +1630,28 @@
         <v>106197010</v>
       </c>
       <c r="D31" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="E31" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="H31" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="E31" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F31" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="G31" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="H31" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I31" s="4" t="n">
+        <v>90</v>
+      </c>
+      <c r="J31" s="4"/>
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B32" s="4" t="n">
         <v>81179582</v>
@@ -1533,24 +1660,28 @@
         <v>81179818</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H32" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>114</v>
+      </c>
+      <c r="I32" s="4" t="n">
+        <v>90</v>
+      </c>
+      <c r="J32" s="4"/>
+    </row>
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="6" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B33" s="6" t="n">
         <v>74327170</v>
@@ -1559,24 +1690,28 @@
         <v>74327374</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F33" s="6" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>114</v>
+      </c>
+      <c r="I33" s="4" t="n">
+        <v>90</v>
+      </c>
+      <c r="J33" s="4"/>
+    </row>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B34" s="4" t="n">
         <v>6419061</v>
@@ -1585,24 +1720,28 @@
         <v>6419298</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H34" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>114</v>
+      </c>
+      <c r="I34" s="4" t="n">
+        <v>90</v>
+      </c>
+      <c r="J34" s="4"/>
+    </row>
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B35" s="6" t="n">
         <v>6418118</v>
@@ -1611,24 +1750,28 @@
         <v>6418330</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="H35" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>114</v>
+      </c>
+      <c r="I35" s="4" t="n">
+        <v>90</v>
+      </c>
+      <c r="J35" s="4"/>
+    </row>
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="4" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B36" s="4" t="n">
         <v>32616720</v>
@@ -1637,24 +1780,28 @@
         <v>32616969</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H36" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>114</v>
+      </c>
+      <c r="I36" s="4" t="n">
+        <v>90</v>
+      </c>
+      <c r="J36" s="4"/>
+    </row>
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B37" s="6" t="n">
         <v>108938384</v>
@@ -1663,24 +1810,28 @@
         <v>108938623</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F37" s="6" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="H37" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>114</v>
+      </c>
+      <c r="I37" s="4" t="n">
+        <v>90</v>
+      </c>
+      <c r="J37" s="4"/>
+    </row>
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B38" s="4" t="n">
         <v>108938000</v>
@@ -1689,24 +1840,28 @@
         <v>108938239</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="H38" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>114</v>
+      </c>
+      <c r="I38" s="4" t="n">
+        <v>90</v>
+      </c>
+      <c r="J38" s="4"/>
+    </row>
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="6" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B39" s="6" t="n">
         <v>32618181</v>
@@ -1715,24 +1870,28 @@
         <v>32618430</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F39" s="6" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="H39" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>114</v>
+      </c>
+      <c r="I39" s="4" t="n">
+        <v>90</v>
+      </c>
+      <c r="J39" s="4"/>
+    </row>
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B40" s="4" t="n">
         <v>81177695</v>
@@ -1741,24 +1900,28 @@
         <v>81177935</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="H40" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>114</v>
+      </c>
+      <c r="I40" s="4" t="n">
+        <v>90</v>
+      </c>
+      <c r="J40" s="4"/>
+    </row>
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="6" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B41" s="6" t="n">
         <v>74332092</v>
@@ -1767,20 +1930,24 @@
         <v>74332336</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F41" s="6" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="G41" s="6" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="H41" s="5" t="s">
-        <v>113</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="I41" s="4" t="n">
+        <v>90</v>
+      </c>
+      <c r="J41" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>